<commit_message>
Début de changement de découpage avec ce qu'il faut rajouter sous le tableau
</commit_message>
<xml_diff>
--- a/DefinitionEtSuiviDeTaches-v02 (1).xlsx
+++ b/DefinitionEtSuiviDeTaches-v02 (1).xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panda/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-i7-Julien\Documents\GitHub\ps5-GroupeK\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{682AB441-7EDD-4BF9-ABBD-EB42AB7BA548}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>Numéro</t>
   </si>
@@ -82,26 +83,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>2cartes + (la paire +la suite de 2 cartes)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>3cartes + (le brelan + la suite de 3 cartes)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>4cartes + (le carré + la double paire + la suite de 4 cartes)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>5cartes + ((le full =la paire + le brelan )+ la suite de 5 cartes)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ajoute Tr Ca Co Pi + la couleur + (Quinte flush = couleur + suite) </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Final</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -146,17 +127,71 @@
   <si>
     <t>12/09</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>19/09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4cartes + le carré </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2cartes + la paire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3cartes + le brelan </t>
+  </si>
+  <si>
+    <t>la suite de 5 cartes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajoute Tr Ca Co Pi + la couleur </t>
+  </si>
+  <si>
+    <t>Quinte flush = couleur + suite</t>
+  </si>
+  <si>
+    <t>suite</t>
+  </si>
+  <si>
+    <t>couleur</t>
+  </si>
+  <si>
+    <t>quinte flush</t>
+  </si>
+  <si>
+    <t>finalisation pour tester que le joueur rentre la bonne synthaxe</t>
+  </si>
+  <si>
+    <t>5cartes + (le full =la paire + le brelan ) + test</t>
+  </si>
+  <si>
+    <t>Hanting  + Julien</t>
+  </si>
+  <si>
+    <t>rajouter pourquoi on gagne</t>
+  </si>
+  <si>
+    <t>rajouter les tests</t>
+  </si>
+  <si>
+    <t>rajouter les cas d'égalité</t>
+  </si>
+  <si>
+    <t>rajouter la synthaxe avant la fin (nombre de cartes)</t>
+  </si>
+  <si>
+    <t>rajouter programme saisie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -165,7 +200,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -173,7 +208,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -181,19 +216,19 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -268,21 +303,21 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="26">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -295,6 +330,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -305,6 +350,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -334,6 +389,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -355,6 +417,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -365,6 +437,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -374,6 +456,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -391,6 +480,16 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -408,147 +507,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -874,41 +838,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="21.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="59.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="34.1640625" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.296875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="59.69921875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.796875" customWidth="1"/>
+    <col min="5" max="5" width="34.19921875" customWidth="1"/>
+    <col min="7" max="7" width="13.796875" customWidth="1"/>
+    <col min="8" max="8" width="12.69921875" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -928,7 +892,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
@@ -940,7 +904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <f>ROW(A3)-2</f>
         <v>1</v>
@@ -952,7 +916,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1">
@@ -961,29 +925,29 @@
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>35</v>
+      <c r="H3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A8" si="0">ROW(A4)-2</f>
+        <f t="shared" ref="A4:A14" si="0">ROW(A4)-2</f>
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
@@ -992,29 +956,29 @@
       <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>34</v>
+      <c r="H4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1">
@@ -1023,27 +987,29 @@
       <c r="G5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="11"/>
+      <c r="H5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
@@ -1052,121 +1018,299 @@
       <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
       <c r="J6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
       <c r="J7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
         <v>5</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
       <c r="J8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    <row r="9" spans="1:10">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
+        <v>6</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <v>7</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1">
+        <v>8</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="7" customFormat="1">
+      <c r="A12" s="1"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" s="7" customFormat="1">
+      <c r="A13" s="1"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="C15" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="C16" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="C17" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="C18" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="C19" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="8">
+    <row r="21" spans="1:3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8">
         <v>1</v>
       </c>
-      <c r="C12" s="9">
-        <f>COUNTIFS($F$3:$F$8,B13,$J$3:$J$8,"=OK")/COUNTIF($F$3:$F$8,B13)</f>
+      <c r="C21" s="9">
+        <f>COUNTIFS($F$3:$F$14,B22,$J$3:$J$14,"=OK")/COUNTIF($F$3:$F$14,B22)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="8">
-        <f>B12+1</f>
+    <row r="22" spans="1:3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8">
+        <f>B21+1</f>
         <v>2</v>
       </c>
-      <c r="C13" s="9">
-        <f t="shared" ref="C13:C14" si="1">COUNTIFS($F$3:$F$8,B14,$J$3:$J$8,"=OK")/COUNTIF($F$3:$F$8,B14)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="6">
+      <c r="C22" s="9">
+        <f t="shared" ref="C22:C29" si="1">COUNTIFS($F$3:$F$14,B23,$J$3:$J$14,"=OK")/COUNTIF($F$3:$F$14,B23)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" s="6">
         <v>3</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C23" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="6">
+    <row r="24" spans="1:3">
+      <c r="B24" s="6">
         <v>4</v>
       </c>
-      <c r="C15" s="9">
-        <f>COUNTIFS($F$3:$F$8,B16,$J$3:$J$8,"=OK")/COUNTIF($F$3:$F$8,B16)</f>
+      <c r="C24" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="6">
+    <row r="25" spans="1:3">
+      <c r="B25" s="6">
         <v>5</v>
       </c>
-      <c r="C16" s="9">
-        <f>COUNTIFS($F$3:$F$8,B17,$J$3:$J$8,"=OK")/COUNTIF($F$3:$F$8,B17)</f>
+      <c r="C25" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="6">
-        <v>5</v>
-      </c>
+    <row r="26" spans="1:3">
+      <c r="B26" s="6">
+        <v>6</v>
+      </c>
+      <c r="C26" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" s="6">
+        <v>7</v>
+      </c>
+      <c r="C27" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28" s="6">
+        <v>8</v>
+      </c>
+      <c r="C28" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" s="6">
+        <v>8</v>
+      </c>
+      <c r="C29" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1174,108 +1318,88 @@
     <mergeCell ref="H1:J1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="PF">
+  <conditionalFormatting sqref="G6:G8">
+    <cfRule type="containsText" dxfId="25" priority="40" operator="containsText" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="24" priority="37" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:G3 B8 D7:F8 D6:G6 A9:G1048576">
-    <cfRule type="cellIs" dxfId="31" priority="37" operator="equal">
+  <conditionalFormatting sqref="A1:G3 D6:G6 A17 C17:G17 B8:B14 D15:G16 G7:G8 A18:G1048576 D7:F14">
+    <cfRule type="cellIs" dxfId="23" priority="41" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:J3 H9:J1048576 I3:I8">
-    <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
+  <conditionalFormatting sqref="H1:J3 H15:J1048576 I3:I4 I6:I14">
+    <cfRule type="cellIs" dxfId="22" priority="38" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="PF">
+    <cfRule type="containsText" dxfId="21" priority="35" operator="containsText" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5">
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:G4 C6:C8 B6:B7 B5:F5">
-    <cfRule type="cellIs" dxfId="27" priority="32" operator="equal">
+  <conditionalFormatting sqref="B4:G4 B6:B7 B5:F5 C6:C14">
+    <cfRule type="cellIs" dxfId="20" priority="36" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
+  <conditionalFormatting sqref="A4:A14">
+    <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6">
+    <cfRule type="containsText" dxfId="18" priority="25" operator="containsText" text="NOK">
+      <formula>NOT(ISERROR(SEARCH("NOK",J6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6">
+    <cfRule type="cellIs" dxfId="17" priority="26" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A8">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+  <conditionalFormatting sqref="J7">
+    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="NOK">
+      <formula>NOT(ISERROR(SEARCH("NOK",J7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7">
+    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8:J14">
+    <cfRule type="containsText" dxfId="14" priority="21" operator="containsText" text="NOK">
+      <formula>NOT(ISERROR(SEARCH("NOK",J8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8:J14">
+    <cfRule type="cellIs" dxfId="13" priority="22" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9 G12:G14">
+    <cfRule type="containsText" dxfId="12" priority="19" operator="containsText" text="PF">
+      <formula>NOT(ISERROR(SEARCH("PF",G9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9 G12:G14">
+    <cfRule type="cellIs" dxfId="11" priority="20" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J6">
-    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J6">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7">
-    <cfRule type="containsText" dxfId="22" priority="19" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J8">
-    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
-    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="PF">
-      <formula>NOT(ISERROR(SEARCH("PF",G8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="PF">
-      <formula>NOT(ISERROR(SEARCH("PF",G7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12:C16">
-    <cfRule type="dataBar" priority="40">
+  <conditionalFormatting sqref="C21:C29">
+    <cfRule type="dataBar" priority="44">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -1287,7 +1411,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="41">
+    <cfRule type="dataBar" priority="45">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1300,24 +1424,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="NOK">
+  <conditionalFormatting sqref="J4:J5">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+  <conditionalFormatting sqref="J4:J5">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H8">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+  <conditionalFormatting sqref="I5 H5:H14">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="PF">
+      <formula>NOT(ISERROR(SEARCH("PF",G10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="PF">
+      <formula>NOT(ISERROR(SEARCH("PF",G11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1348,7 +1492,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C12:C16</xm:sqref>
+          <xm:sqref>C21:C29</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>